<commit_message>
repairing of ifc models / changing attribute values implemented
</commit_message>
<xml_diff>
--- a/projects/002_example_project__public/buildings/test_building_001/04_metrics/test_building_001_metrics.xlsx
+++ b/projects/002_example_project__public/buildings/test_building_001/04_metrics/test_building_001_metrics.xlsx
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>45772.62694637835</v>
+        <v>45772.8877075925</v>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="F3" s="4" t="n">
-        <v>45772.62694691433</v>
+        <v>45772.88770819711</v>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="F4" s="4" t="n">
-        <v>45772.62694747296</v>
+        <v>45772.88770873848</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="F5" s="4" t="n">
-        <v>45772.62694797976</v>
+        <v>45772.88770927358</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="F6" s="4" t="n">
-        <v>45772.6269485204</v>
+        <v>45772.88770981528</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F7" s="4" t="n">
-        <v>45772.62694906976</v>
+        <v>45772.88771037861</v>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="F8" s="4" t="n">
-        <v>45772.62694961302</v>
+        <v>45772.88771095581</v>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
@@ -761,7 +761,7 @@
         </is>
       </c>
       <c r="F9" s="4" t="n">
-        <v>45772.62695018652</v>
+        <v>45772.88771157902</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="F10" s="4" t="n">
-        <v>45772.62695075295</v>
+        <v>45772.88771223522</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="F11" s="4" t="n">
-        <v>45772.62695129942</v>
+        <v>45772.88771280439</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="F12" s="4" t="n">
-        <v>45772.62695183111</v>
+        <v>45772.88771335773</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="F13" s="4" t="n">
-        <v>45772.62695239203</v>
+        <v>45772.88771392005</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="F14" s="4" t="n">
-        <v>45772.6269529497</v>
+        <v>45772.88771449949</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="F15" s="4" t="n">
-        <v>45772.62695346927</v>
+        <v>45772.88771503014</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="F16" s="4" t="n">
-        <v>45772.62695399306</v>
+        <v>45772.88771556409</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="F17" s="4" t="n">
-        <v>45772.62695452338</v>
+        <v>45772.88771610897</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="F18" s="4" t="n">
-        <v>45772.62695504494</v>
+        <v>45772.8877167542</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="F19" s="4" t="n">
-        <v>45772.62695557863</v>
+        <v>45772.88771744322</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="F20" s="4" t="n">
-        <v>45772.62695612261</v>
+        <v>45772.88771796894</v>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="F21" s="4" t="n">
-        <v>45772.62695665368</v>
+        <v>45772.88771850441</v>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="F22" s="4" t="n">
-        <v>45772.62695724042</v>
+        <v>45772.88771908221</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
@@ -1223,7 +1223,7 @@
         </is>
       </c>
       <c r="F23" s="4" t="n">
-        <v>45772.6269578916</v>
+        <v>45772.88771972692</v>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="F24" s="4" t="n">
-        <v>45772.62695851729</v>
+        <v>45772.88772039859</v>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="F25" s="4" t="n">
-        <v>45772.62695932446</v>
+        <v>45772.8877211955</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="F26" s="4" t="n">
-        <v>45772.62696028459</v>
+        <v>45772.88772213501</v>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>45772.62696172957</v>
+        <v>45772.88772303401</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
@@ -1388,7 +1388,7 @@
         </is>
       </c>
       <c r="F28" s="4" t="n">
-        <v>45772.62696253113</v>
+        <v>45772.88772376999</v>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
@@ -1421,7 +1421,7 @@
         </is>
       </c>
       <c r="F29" s="4" t="n">
-        <v>45772.62696387647</v>
+        <v>45772.88772513199</v>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="F30" s="4" t="n">
-        <v>45772.62696531085</v>
+        <v>45772.88772624217</v>
       </c>
       <c r="G30" s="2" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="F31" s="4" t="n">
-        <v>45772.62696624396</v>
+        <v>45772.88772706065</v>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F32" s="4" t="n">
-        <v>45772.62696684955</v>
+        <v>45772.88772758836</v>
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
@@ -1556,7 +1556,7 @@
         </is>
       </c>
       <c r="F33" s="4" t="n">
-        <v>45772.6269674385</v>
+        <v>45772.88772809969</v>
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="F34" s="4" t="n">
-        <v>45772.62696805274</v>
+        <v>45772.88772861967</v>
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="F35" s="4" t="n">
-        <v>45772.6269686637</v>
+        <v>45772.88772914097</v>
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         </is>
       </c>
       <c r="F36" s="4" t="n">
-        <v>45772.62696925402</v>
+        <v>45772.88772965258</v>
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
         </is>
       </c>
       <c r="F37" s="4" t="n">
-        <v>45772.62696989105</v>
+        <v>45772.88773017472</v>
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
@@ -1721,7 +1721,7 @@
         </is>
       </c>
       <c r="F38" s="4" t="n">
-        <v>45772.62697051047</v>
+        <v>45772.88773069469</v>
       </c>
       <c r="G38" s="2" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="F39" s="4" t="n">
-        <v>45772.62697106371</v>
+        <v>45772.88773121977</v>
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="F40" s="4" t="n">
-        <v>45772.62697162681</v>
+        <v>45772.88773174757</v>
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="F41" s="4" t="n">
-        <v>45772.62697220813</v>
+        <v>45772.88773228028</v>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="F42" s="4" t="n">
-        <v>45772.62697279523</v>
+        <v>45772.88773290956</v>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F43" s="4" t="n">
-        <v>45772.62697329802</v>
+        <v>45772.88773347543</v>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="F44" s="4" t="n">
-        <v>45772.62697382725</v>
+        <v>45772.88773400019</v>
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="F45" s="4" t="n">
-        <v>45772.62697438645</v>
+        <v>45772.88773451289</v>
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="F46" s="4" t="n">
-        <v>45772.62697495946</v>
+        <v>45772.88773503348</v>
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="F47" s="4" t="n">
-        <v>45772.62697552262</v>
+        <v>45772.88773554294</v>
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="F48" s="4" t="n">
-        <v>45772.62697609334</v>
+        <v>45772.88773605476</v>
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="F49" s="4" t="n">
-        <v>45772.62697673177</v>
+        <v>45772.88773663968</v>
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="F50" s="4" t="n">
-        <v>45772.62697742567</v>
+        <v>45772.88773729102</v>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="F51" s="4" t="n">
-        <v>45772.62697813252</v>
+        <v>45772.88773794261</v>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
@@ -2188,7 +2188,7 @@
         </is>
       </c>
       <c r="F52" s="4" t="n">
-        <v>45772.62697878274</v>
+        <v>45772.88773856989</v>
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
@@ -2225,7 +2225,7 @@
         </is>
       </c>
       <c r="F53" s="4" t="n">
-        <v>45772.62697949701</v>
+        <v>45772.88773921559</v>
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="F54" s="4" t="n">
-        <v>45772.6269802055</v>
+        <v>45772.88773985129</v>
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="F55" s="4" t="n">
-        <v>45772.62698078589</v>
+        <v>45772.8877403974</v>
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="F56" s="4" t="n">
-        <v>45772.62698134447</v>
+        <v>45772.88774092392</v>
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
@@ -2361,7 +2361,7 @@
         </is>
       </c>
       <c r="F57" s="4" t="n">
-        <v>45772.62698190725</v>
+        <v>45772.88774144904</v>
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
@@ -2394,7 +2394,7 @@
         </is>
       </c>
       <c r="F58" s="4" t="n">
-        <v>45772.62698246048</v>
+        <v>45772.88774198217</v>
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="F59" s="4" t="n">
-        <v>45772.62698246063</v>
+        <v>45772.88774198237</v>
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="E60" s="2" t="inlineStr"/>
       <c r="F60" s="4" t="n">
-        <v>45772.6269838191</v>
+        <v>45772.88774322515</v>
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="E61" s="2" t="inlineStr"/>
       <c r="F61" s="4" t="n">
-        <v>45772.62698472526</v>
+        <v>45772.88774409903</v>
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
@@ -2514,7 +2514,7 @@
         </is>
       </c>
       <c r="F62" s="4" t="n">
-        <v>45772.62698532594</v>
+        <v>45772.88774479157</v>
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
@@ -2547,7 +2547,7 @@
         </is>
       </c>
       <c r="F63" s="4" t="n">
-        <v>45772.62698532604</v>
+        <v>45772.88774479173</v>
       </c>
       <c r="G63" s="2" t="inlineStr">
         <is>
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="F64" s="4" t="n">
-        <v>45772.62698532607</v>
+        <v>45772.88774479175</v>
       </c>
       <c r="G64" s="2" t="inlineStr">
         <is>
@@ -2613,7 +2613,7 @@
         </is>
       </c>
       <c r="F65" s="4" t="n">
-        <v>45772.62698532607</v>
+        <v>45772.88774479176</v>
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
@@ -2646,7 +2646,7 @@
         </is>
       </c>
       <c r="F66" s="4" t="n">
-        <v>45772.62698532609</v>
+        <v>45772.88774479177</v>
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
@@ -2679,7 +2679,7 @@
         </is>
       </c>
       <c r="F67" s="4" t="n">
-        <v>45772.62698532611</v>
+        <v>45772.88774479179</v>
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="F68" s="4" t="n">
-        <v>45772.62698532613</v>
+        <v>45772.88774479181</v>
       </c>
       <c r="G68" s="2" t="inlineStr">
         <is>
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="F69" s="4" t="n">
-        <v>45772.62698532618</v>
+        <v>45772.88774479186</v>
       </c>
       <c r="G69" s="2" t="inlineStr">
         <is>
@@ -2778,7 +2778,7 @@
         </is>
       </c>
       <c r="F70" s="4" t="n">
-        <v>45772.62698532621</v>
+        <v>45772.88774479199</v>
       </c>
       <c r="G70" s="2" t="inlineStr">
         <is>
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="F71" s="4" t="n">
-        <v>45772.62698532631</v>
+        <v>45772.887744792</v>
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
@@ -2844,7 +2844,7 @@
         </is>
       </c>
       <c r="F72" s="4" t="n">
-        <v>45772.62698532632</v>
+        <v>45772.88774479202</v>
       </c>
       <c r="G72" s="2" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="F73" s="4" t="n">
-        <v>45772.62698532633</v>
+        <v>45772.88774479202</v>
       </c>
       <c r="G73" s="2" t="inlineStr">
         <is>
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="F74" s="4" t="n">
-        <v>45772.62698591625</v>
+        <v>45772.88774540508</v>
       </c>
       <c r="G74" s="2" t="inlineStr">
         <is>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="F75" s="4" t="n">
-        <v>45772.62698591635</v>
+        <v>45772.88774540518</v>
       </c>
       <c r="G75" s="2" t="inlineStr">
         <is>
@@ -2976,7 +2976,7 @@
         </is>
       </c>
       <c r="F76" s="4" t="n">
-        <v>45772.62698591638</v>
+        <v>45772.8877454052</v>
       </c>
       <c r="G76" s="2" t="inlineStr">
         <is>
@@ -3009,7 +3009,7 @@
         </is>
       </c>
       <c r="F77" s="4" t="n">
-        <v>45772.62698591639</v>
+        <v>45772.88774540521</v>
       </c>
       <c r="G77" s="2" t="inlineStr">
         <is>
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="F78" s="4" t="n">
-        <v>45772.62698591641</v>
+        <v>45772.88774540522</v>
       </c>
       <c r="G78" s="2" t="inlineStr">
         <is>
@@ -3075,7 +3075,7 @@
         </is>
       </c>
       <c r="F79" s="4" t="n">
-        <v>45772.62698591642</v>
+        <v>45772.88774540523</v>
       </c>
       <c r="G79" s="2" t="inlineStr">
         <is>
@@ -3108,7 +3108,7 @@
         </is>
       </c>
       <c r="F80" s="4" t="n">
-        <v>45772.62698591644</v>
+        <v>45772.88774540524</v>
       </c>
       <c r="G80" s="2" t="inlineStr">
         <is>
@@ -3141,7 +3141,7 @@
         </is>
       </c>
       <c r="F81" s="4" t="n">
-        <v>45772.62698591645</v>
+        <v>45772.88774540526</v>
       </c>
       <c r="G81" s="2" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
         </is>
       </c>
       <c r="F82" s="4" t="n">
-        <v>45772.62698591646</v>
+        <v>45772.88774540526</v>
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="F83" s="4" t="n">
-        <v>45772.62698591647</v>
+        <v>45772.88774540528</v>
       </c>
       <c r="G83" s="2" t="inlineStr">
         <is>
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="F84" s="4" t="n">
-        <v>45772.62698591648</v>
+        <v>45772.88774540529</v>
       </c>
       <c r="G84" s="2" t="inlineStr">
         <is>
@@ -3273,7 +3273,7 @@
         </is>
       </c>
       <c r="F85" s="4" t="n">
-        <v>45772.62698591649</v>
+        <v>45772.8877454053</v>
       </c>
       <c r="G85" s="2" t="inlineStr">
         <is>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="E86" s="2" t="inlineStr"/>
       <c r="F86" s="4" t="n">
-        <v>45772.62698718064</v>
+        <v>45772.88774669853</v>
       </c>
       <c r="G86" s="2" t="inlineStr">
         <is>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="E87" s="2" t="inlineStr"/>
       <c r="F87" s="4" t="n">
-        <v>45772.6269877954</v>
+        <v>45772.88774730165</v>
       </c>
       <c r="G87" s="2" t="inlineStr">
         <is>
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="F88" s="4" t="n">
-        <v>45772.62698801161</v>
+        <v>45772.88774750574</v>
       </c>
       <c r="G88" s="2" t="inlineStr">
         <is>
@@ -3393,7 +3393,7 @@
         </is>
       </c>
       <c r="F89" s="4" t="n">
-        <v>45772.62698803481</v>
+        <v>45772.88774752941</v>
       </c>
       <c r="G89" s="2" t="inlineStr">
         <is>
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="F90" s="4" t="n">
-        <v>45772.62698805571</v>
+        <v>45772.88774754895</v>
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
@@ -3459,7 +3459,7 @@
         </is>
       </c>
       <c r="F91" s="4" t="n">
-        <v>45772.62698807586</v>
+        <v>45772.8877475686</v>
       </c>
       <c r="G91" s="2" t="inlineStr">
         <is>
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="F92" s="4" t="n">
-        <v>45772.6269880957</v>
+        <v>45772.88774758817</v>
       </c>
       <c r="G92" s="2" t="inlineStr">
         <is>
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="F93" s="4" t="n">
-        <v>45772.62698811521</v>
+        <v>45772.88774760756</v>
       </c>
       <c r="G93" s="2" t="inlineStr">
         <is>
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="F94" s="4" t="n">
-        <v>45772.62698813483</v>
+        <v>45772.8877476268</v>
       </c>
       <c r="G94" s="2" t="inlineStr">
         <is>
@@ -3591,7 +3591,7 @@
         </is>
       </c>
       <c r="F95" s="4" t="n">
-        <v>45772.62698815432</v>
+        <v>45772.88774764598</v>
       </c>
       <c r="G95" s="2" t="inlineStr">
         <is>
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="F96" s="4" t="n">
-        <v>45772.62698817319</v>
+        <v>45772.88774766524</v>
       </c>
       <c r="G96" s="2" t="inlineStr">
         <is>
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="F97" s="4" t="n">
-        <v>45772.62698819202</v>
+        <v>45772.88774768436</v>
       </c>
       <c r="G97" s="2" t="inlineStr">
         <is>
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="F98" s="4" t="n">
-        <v>45772.62698821085</v>
+        <v>45772.88774770327</v>
       </c>
       <c r="G98" s="2" t="inlineStr">
         <is>
@@ -3723,7 +3723,7 @@
         </is>
       </c>
       <c r="F99" s="4" t="n">
-        <v>45772.62698822962</v>
+        <v>45772.88774772194</v>
       </c>
       <c r="G99" s="2" t="inlineStr">
         <is>
@@ -3756,7 +3756,7 @@
         </is>
       </c>
       <c r="F100" s="4" t="n">
-        <v>45772.62698824907</v>
+        <v>45772.88774774069</v>
       </c>
       <c r="G100" s="2" t="inlineStr">
         <is>
@@ -3789,7 +3789,7 @@
         </is>
       </c>
       <c r="F101" s="4" t="n">
-        <v>45772.62698826924</v>
+        <v>45772.88774775965</v>
       </c>
       <c r="G101" s="2" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F102" s="4" t="n">
-        <v>45772.6269882874</v>
+        <v>45772.88774777844</v>
       </c>
       <c r="G102" s="2" t="inlineStr">
         <is>
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="F103" s="4" t="n">
-        <v>45772.62698830539</v>
+        <v>45772.88774779691</v>
       </c>
       <c r="G103" s="2" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
         </is>
       </c>
       <c r="F104" s="4" t="n">
-        <v>45772.62698832354</v>
+        <v>45772.88774781552</v>
       </c>
       <c r="G104" s="2" t="inlineStr">
         <is>
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="F105" s="4" t="n">
-        <v>45772.62698834185</v>
+        <v>45772.88774783398</v>
       </c>
       <c r="G105" s="2" t="inlineStr">
         <is>
@@ -3954,7 +3954,7 @@
         </is>
       </c>
       <c r="F106" s="4" t="n">
-        <v>45772.62698835995</v>
+        <v>45772.88774785215</v>
       </c>
       <c r="G106" s="2" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
         </is>
       </c>
       <c r="F107" s="4" t="n">
-        <v>45772.62698837837</v>
+        <v>45772.88774787167</v>
       </c>
       <c r="G107" s="2" t="inlineStr">
         <is>
@@ -4020,7 +4020,7 @@
         </is>
       </c>
       <c r="F108" s="4" t="n">
-        <v>45772.62698839657</v>
+        <v>45772.88774789015</v>
       </c>
       <c r="G108" s="2" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
         </is>
       </c>
       <c r="F109" s="4" t="n">
-        <v>45772.62698841523</v>
+        <v>45772.88774791663</v>
       </c>
       <c r="G109" s="2" t="inlineStr">
         <is>
@@ -4086,7 +4086,7 @@
         </is>
       </c>
       <c r="F110" s="4" t="n">
-        <v>45772.62698843364</v>
+        <v>45772.88774793562</v>
       </c>
       <c r="G110" s="2" t="inlineStr">
         <is>
@@ -4119,7 +4119,7 @@
         </is>
       </c>
       <c r="F111" s="4" t="n">
-        <v>45772.62698845188</v>
+        <v>45772.88774795782</v>
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="F112" s="4" t="n">
-        <v>45772.62698846999</v>
+        <v>45772.88774797876</v>
       </c>
       <c r="G112" s="2" t="inlineStr">
         <is>
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="F113" s="4" t="n">
-        <v>45772.62698848832</v>
+        <v>45772.8877479975</v>
       </c>
       <c r="G113" s="2" t="inlineStr">
         <is>
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="F114" s="4" t="n">
-        <v>45772.62698850654</v>
+        <v>45772.88774801591</v>
       </c>
       <c r="G114" s="2" t="inlineStr">
         <is>
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="F115" s="4" t="n">
-        <v>45772.62698852465</v>
+        <v>45772.88774803425</v>
       </c>
       <c r="G115" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
code is a big mess, sorry for not creating a branche.just thought a quick fix...
</commit_message>
<xml_diff>
--- a/projects/002_example_project__public/buildings/test_building_001/04_metrics/test_building_001_metrics.xlsx
+++ b/projects/002_example_project__public/buildings/test_building_001/04_metrics/test_building_001_metrics.xlsx
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>45772.94156683885</v>
+        <v>45773.9126282363</v>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="F3" s="4" t="n">
-        <v>45772.94156739787</v>
+        <v>45773.91262875602</v>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="F4" s="4" t="n">
-        <v>45772.94156809262</v>
+        <v>45773.91262928458</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="F5" s="4" t="n">
-        <v>45772.94156860264</v>
+        <v>45773.9126297759</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="F6" s="4" t="n">
-        <v>45772.94156912946</v>
+        <v>45773.91263029215</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F7" s="4" t="n">
-        <v>45772.94156965793</v>
+        <v>45773.9126308124</v>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="F8" s="4" t="n">
-        <v>45772.94157017388</v>
+        <v>45773.91263131925</v>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
@@ -761,7 +761,7 @@
         </is>
       </c>
       <c r="F9" s="4" t="n">
-        <v>45772.94157074861</v>
+        <v>45773.91263186544</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="F10" s="4" t="n">
-        <v>45772.94157132204</v>
+        <v>45773.91263241286</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="F11" s="4" t="n">
-        <v>45772.94157184015</v>
+        <v>45773.91263292476</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="F12" s="4" t="n">
-        <v>45772.94157234835</v>
+        <v>45773.91263342176</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="F13" s="4" t="n">
-        <v>45772.94157290245</v>
+        <v>45773.9126339538</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="F14" s="4" t="n">
-        <v>45772.94157344435</v>
+        <v>45773.91263447842</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="F15" s="4" t="n">
-        <v>45772.94157397703</v>
+        <v>45773.91263496603</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="F16" s="4" t="n">
-        <v>45772.94157451415</v>
+        <v>45773.91263545559</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="F17" s="4" t="n">
-        <v>45772.94157503577</v>
+        <v>45773.91263594059</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="F18" s="4" t="n">
-        <v>45772.94157556324</v>
+        <v>45773.9126364302</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="F19" s="4" t="n">
-        <v>45772.94157609899</v>
+        <v>45773.91263692616</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="F20" s="4" t="n">
-        <v>45772.94157663071</v>
+        <v>45773.91263742017</v>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="F21" s="4" t="n">
-        <v>45772.94157716983</v>
+        <v>45773.9126379204</v>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="F22" s="4" t="n">
-        <v>45772.94157775905</v>
+        <v>45773.91263846097</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
@@ -1223,7 +1223,7 @@
         </is>
       </c>
       <c r="F23" s="4" t="n">
-        <v>45772.94157842181</v>
+        <v>45773.91263906474</v>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="F24" s="4" t="n">
-        <v>45772.94157906765</v>
+        <v>45773.91263967872</v>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="F25" s="4" t="n">
-        <v>45772.94157992135</v>
+        <v>45773.91264050485</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="F26" s="4" t="n">
-        <v>45772.94158094377</v>
+        <v>45773.91264269219</v>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>45772.9415819489</v>
+        <v>45773.91264364828</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
@@ -1388,7 +1388,7 @@
         </is>
       </c>
       <c r="F28" s="4" t="n">
-        <v>45772.94158302545</v>
+        <v>45773.91264439347</v>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
@@ -1421,7 +1421,7 @@
         </is>
       </c>
       <c r="F29" s="4" t="n">
-        <v>45772.9415840145</v>
+        <v>45773.9126453016</v>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="F30" s="4" t="n">
-        <v>45772.94158493647</v>
+        <v>45773.91264620119</v>
       </c>
       <c r="G30" s="2" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="F31" s="4" t="n">
-        <v>45772.9415856988</v>
+        <v>45773.91264696535</v>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F32" s="4" t="n">
-        <v>45772.94158623516</v>
+        <v>45773.91264752953</v>
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
@@ -1556,7 +1556,7 @@
         </is>
       </c>
       <c r="F33" s="4" t="n">
-        <v>45772.94158674772</v>
+        <v>45773.91264802944</v>
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="F34" s="4" t="n">
-        <v>45772.94158727969</v>
+        <v>45773.91264854317</v>
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="F35" s="4" t="n">
-        <v>45772.94158779824</v>
+        <v>45773.91264905013</v>
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         </is>
       </c>
       <c r="F36" s="4" t="n">
-        <v>45772.94158831875</v>
+        <v>45773.91264955245</v>
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
         </is>
       </c>
       <c r="F37" s="4" t="n">
-        <v>45772.94158884726</v>
+        <v>45773.91265006747</v>
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
@@ -1721,7 +1721,7 @@
         </is>
       </c>
       <c r="F38" s="4" t="n">
-        <v>45772.94158937135</v>
+        <v>45773.91265058192</v>
       </c>
       <c r="G38" s="2" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="F39" s="4" t="n">
-        <v>45772.94158989096</v>
+        <v>45773.91265107925</v>
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="F40" s="4" t="n">
-        <v>45772.94159042164</v>
+        <v>45773.91265159703</v>
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="F41" s="4" t="n">
-        <v>45772.94159096344</v>
+        <v>45773.91265211068</v>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="F42" s="4" t="n">
-        <v>45772.94159147557</v>
+        <v>45773.91265261287</v>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F43" s="4" t="n">
-        <v>45772.94159198929</v>
+        <v>45773.91265311016</v>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="F44" s="4" t="n">
-        <v>45772.9415925038</v>
+        <v>45773.91265360954</v>
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="F45" s="4" t="n">
-        <v>45772.94159302111</v>
+        <v>45773.91265410541</v>
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="F46" s="4" t="n">
-        <v>45772.94159353766</v>
+        <v>45773.91265460493</v>
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="F47" s="4" t="n">
-        <v>45772.94159405136</v>
+        <v>45773.91265509769</v>
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="F48" s="4" t="n">
-        <v>45772.94159456853</v>
+        <v>45773.91265559488</v>
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="F49" s="4" t="n">
-        <v>45772.94159514196</v>
+        <v>45773.91265615854</v>
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="F50" s="4" t="n">
-        <v>45772.94159578221</v>
+        <v>45773.91265693743</v>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="F51" s="4" t="n">
-        <v>45772.94159642996</v>
+        <v>45773.91265758663</v>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
@@ -2188,7 +2188,7 @@
         </is>
       </c>
       <c r="F52" s="4" t="n">
-        <v>45772.94159702795</v>
+        <v>45773.91265816594</v>
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
@@ -2225,7 +2225,7 @@
         </is>
       </c>
       <c r="F53" s="4" t="n">
-        <v>45772.94159766554</v>
+        <v>45773.91265886419</v>
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="F54" s="4" t="n">
-        <v>45772.94159830564</v>
+        <v>45773.91265960685</v>
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="F55" s="4" t="n">
-        <v>45772.94159886545</v>
+        <v>45773.91266012248</v>
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="F56" s="4" t="n">
-        <v>45772.94159937919</v>
+        <v>45773.91266062044</v>
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
@@ -2361,7 +2361,7 @@
         </is>
       </c>
       <c r="F57" s="4" t="n">
-        <v>45772.94159988585</v>
+        <v>45773.9126611179</v>
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
@@ -2394,7 +2394,7 @@
         </is>
       </c>
       <c r="F58" s="4" t="n">
-        <v>45772.94160042404</v>
+        <v>45773.91266163401</v>
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="F59" s="4" t="n">
-        <v>45772.94160042422</v>
+        <v>45773.91266163419</v>
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="E60" s="2" t="inlineStr"/>
       <c r="F60" s="4" t="n">
-        <v>45772.94160175136</v>
+        <v>45773.91266240962</v>
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="E61" s="2" t="inlineStr"/>
       <c r="F61" s="4" t="n">
-        <v>45772.94160270992</v>
+        <v>45773.91266325641</v>
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
@@ -2514,7 +2514,7 @@
         </is>
       </c>
       <c r="F62" s="4" t="n">
-        <v>45772.94160334452</v>
+        <v>45773.91266387749</v>
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
@@ -2547,7 +2547,7 @@
         </is>
       </c>
       <c r="F63" s="4" t="n">
-        <v>45772.94160334463</v>
+        <v>45773.91266387759</v>
       </c>
       <c r="G63" s="2" t="inlineStr">
         <is>
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="F64" s="4" t="n">
-        <v>45772.94160334465</v>
+        <v>45773.91266387761</v>
       </c>
       <c r="G64" s="2" t="inlineStr">
         <is>
@@ -2613,7 +2613,7 @@
         </is>
       </c>
       <c r="F65" s="4" t="n">
-        <v>45772.94160334466</v>
+        <v>45773.91266387763</v>
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
@@ -2646,7 +2646,7 @@
         </is>
       </c>
       <c r="F66" s="4" t="n">
-        <v>45772.94160334469</v>
+        <v>45773.91266387764</v>
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
@@ -2679,7 +2679,7 @@
         </is>
       </c>
       <c r="F67" s="4" t="n">
-        <v>45772.9416033447</v>
+        <v>45773.91266387765</v>
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="F68" s="4" t="n">
-        <v>45772.94160334471</v>
+        <v>45773.91266387767</v>
       </c>
       <c r="G68" s="2" t="inlineStr">
         <is>
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="F69" s="4" t="n">
-        <v>45772.94160334477</v>
+        <v>45773.91266387773</v>
       </c>
       <c r="G69" s="2" t="inlineStr">
         <is>
@@ -2778,7 +2778,7 @@
         </is>
       </c>
       <c r="F70" s="4" t="n">
-        <v>45772.94160334479</v>
+        <v>45773.91266387775</v>
       </c>
       <c r="G70" s="2" t="inlineStr">
         <is>
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="F71" s="4" t="n">
-        <v>45772.94160334489</v>
+        <v>45773.91266387777</v>
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
@@ -2844,7 +2844,7 @@
         </is>
       </c>
       <c r="F72" s="4" t="n">
-        <v>45772.94160334491</v>
+        <v>45773.91266387777</v>
       </c>
       <c r="G72" s="2" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="F73" s="4" t="n">
-        <v>45772.94160334492</v>
+        <v>45773.91266387779</v>
       </c>
       <c r="G73" s="2" t="inlineStr">
         <is>
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="F74" s="4" t="n">
-        <v>45772.94160390924</v>
+        <v>45773.91266443131</v>
       </c>
       <c r="G74" s="2" t="inlineStr">
         <is>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="F75" s="4" t="n">
-        <v>45772.94160390935</v>
+        <v>45773.91266443139</v>
       </c>
       <c r="G75" s="2" t="inlineStr">
         <is>
@@ -2976,7 +2976,7 @@
         </is>
       </c>
       <c r="F76" s="4" t="n">
-        <v>45772.94160390936</v>
+        <v>45773.9126644314</v>
       </c>
       <c r="G76" s="2" t="inlineStr">
         <is>
@@ -3009,7 +3009,7 @@
         </is>
       </c>
       <c r="F77" s="4" t="n">
-        <v>45772.94160390938</v>
+        <v>45773.91266443141</v>
       </c>
       <c r="G77" s="2" t="inlineStr">
         <is>
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="F78" s="4" t="n">
-        <v>45772.94160390938</v>
+        <v>45773.91266443142</v>
       </c>
       <c r="G78" s="2" t="inlineStr">
         <is>
@@ -3075,7 +3075,7 @@
         </is>
       </c>
       <c r="F79" s="4" t="n">
-        <v>45772.9416039094</v>
+        <v>45773.91266443144</v>
       </c>
       <c r="G79" s="2" t="inlineStr">
         <is>
@@ -3108,7 +3108,7 @@
         </is>
       </c>
       <c r="F80" s="4" t="n">
-        <v>45772.94160390941</v>
+        <v>45773.91266443145</v>
       </c>
       <c r="G80" s="2" t="inlineStr">
         <is>
@@ -3141,7 +3141,7 @@
         </is>
       </c>
       <c r="F81" s="4" t="n">
-        <v>45772.94160390942</v>
+        <v>45773.91266443146</v>
       </c>
       <c r="G81" s="2" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
         </is>
       </c>
       <c r="F82" s="4" t="n">
-        <v>45772.94160390944</v>
+        <v>45773.91266443147</v>
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="F83" s="4" t="n">
-        <v>45772.94160390944</v>
+        <v>45773.91266443148</v>
       </c>
       <c r="G83" s="2" t="inlineStr">
         <is>
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="F84" s="4" t="n">
-        <v>45772.94160390944</v>
+        <v>45773.9126644315</v>
       </c>
       <c r="G84" s="2" t="inlineStr">
         <is>
@@ -3273,7 +3273,7 @@
         </is>
       </c>
       <c r="F85" s="4" t="n">
-        <v>45772.94160390946</v>
+        <v>45773.9126644315</v>
       </c>
       <c r="G85" s="2" t="inlineStr">
         <is>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="E86" s="2" t="inlineStr"/>
       <c r="F86" s="4" t="n">
-        <v>45772.94160514861</v>
+        <v>45773.91266565309</v>
       </c>
       <c r="G86" s="2" t="inlineStr">
         <is>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="E87" s="2" t="inlineStr"/>
       <c r="F87" s="4" t="n">
-        <v>45772.94160578971</v>
+        <v>45773.9126662257</v>
       </c>
       <c r="G87" s="2" t="inlineStr">
         <is>
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="F88" s="4" t="n">
-        <v>45772.94160598635</v>
+        <v>45773.91266689355</v>
       </c>
       <c r="G88" s="2" t="inlineStr">
         <is>
@@ -3393,7 +3393,7 @@
         </is>
       </c>
       <c r="F89" s="4" t="n">
-        <v>45772.94160600991</v>
+        <v>45773.91266691661</v>
       </c>
       <c r="G89" s="2" t="inlineStr">
         <is>
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="F90" s="4" t="n">
-        <v>45772.94160603127</v>
+        <v>45773.91266693729</v>
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
@@ -3459,7 +3459,7 @@
         </is>
       </c>
       <c r="F91" s="4" t="n">
-        <v>45772.94160605163</v>
+        <v>45773.91266695712</v>
       </c>
       <c r="G91" s="2" t="inlineStr">
         <is>
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="F92" s="4" t="n">
-        <v>45772.94160607181</v>
+        <v>45773.91266697707</v>
       </c>
       <c r="G92" s="2" t="inlineStr">
         <is>
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="F93" s="4" t="n">
-        <v>45772.94160609229</v>
+        <v>45773.91266699648</v>
       </c>
       <c r="G93" s="2" t="inlineStr">
         <is>
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="F94" s="4" t="n">
-        <v>45772.94160611273</v>
+        <v>45773.91266701606</v>
       </c>
       <c r="G94" s="2" t="inlineStr">
         <is>
@@ -3591,7 +3591,7 @@
         </is>
       </c>
       <c r="F95" s="4" t="n">
-        <v>45772.94160613319</v>
+        <v>45773.91266703577</v>
       </c>
       <c r="G95" s="2" t="inlineStr">
         <is>
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="F96" s="4" t="n">
-        <v>45772.94160615309</v>
+        <v>45773.91266705455</v>
       </c>
       <c r="G96" s="2" t="inlineStr">
         <is>
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="F97" s="4" t="n">
-        <v>45772.94160617258</v>
+        <v>45773.91266707351</v>
       </c>
       <c r="G97" s="2" t="inlineStr">
         <is>
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="F98" s="4" t="n">
-        <v>45772.94160619185</v>
+        <v>45773.9126670922</v>
       </c>
       <c r="G98" s="2" t="inlineStr">
         <is>
@@ -3723,7 +3723,7 @@
         </is>
       </c>
       <c r="F99" s="4" t="n">
-        <v>45772.94160621176</v>
+        <v>45773.91266711154</v>
       </c>
       <c r="G99" s="2" t="inlineStr">
         <is>
@@ -3756,7 +3756,7 @@
         </is>
       </c>
       <c r="F100" s="4" t="n">
-        <v>45772.94160623087</v>
+        <v>45773.91266713069</v>
       </c>
       <c r="G100" s="2" t="inlineStr">
         <is>
@@ -3789,7 +3789,7 @@
         </is>
       </c>
       <c r="F101" s="4" t="n">
-        <v>45772.94160625054</v>
+        <v>45773.91266714923</v>
       </c>
       <c r="G101" s="2" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F102" s="4" t="n">
-        <v>45772.9416062696</v>
+        <v>45773.91266716787</v>
       </c>
       <c r="G102" s="2" t="inlineStr">
         <is>
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="F103" s="4" t="n">
-        <v>45772.94160628906</v>
+        <v>45773.91266718714</v>
       </c>
       <c r="G103" s="2" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
         </is>
       </c>
       <c r="F104" s="4" t="n">
-        <v>45772.94160630825</v>
+        <v>45773.91266720785</v>
       </c>
       <c r="G104" s="2" t="inlineStr">
         <is>
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="F105" s="4" t="n">
-        <v>45772.94160632673</v>
+        <v>45773.91266722714</v>
       </c>
       <c r="G105" s="2" t="inlineStr">
         <is>
@@ -3954,7 +3954,7 @@
         </is>
       </c>
       <c r="F106" s="4" t="n">
-        <v>45772.94160634507</v>
+        <v>45773.91266724555</v>
       </c>
       <c r="G106" s="2" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
         </is>
       </c>
       <c r="F107" s="4" t="n">
-        <v>45772.94160636391</v>
+        <v>45773.91266726385</v>
       </c>
       <c r="G107" s="2" t="inlineStr">
         <is>
@@ -4020,7 +4020,7 @@
         </is>
       </c>
       <c r="F108" s="4" t="n">
-        <v>45772.94160638242</v>
+        <v>45773.91266728217</v>
       </c>
       <c r="G108" s="2" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
         </is>
       </c>
       <c r="F109" s="4" t="n">
-        <v>45772.94160640085</v>
+        <v>45773.91266730044</v>
       </c>
       <c r="G109" s="2" t="inlineStr">
         <is>
@@ -4086,7 +4086,7 @@
         </is>
       </c>
       <c r="F110" s="4" t="n">
-        <v>45772.94160641933</v>
+        <v>45773.9126673189</v>
       </c>
       <c r="G110" s="2" t="inlineStr">
         <is>
@@ -4119,7 +4119,7 @@
         </is>
       </c>
       <c r="F111" s="4" t="n">
-        <v>45772.94160643787</v>
+        <v>45773.91266733744</v>
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="F112" s="4" t="n">
-        <v>45772.94160645646</v>
+        <v>45773.91266735609</v>
       </c>
       <c r="G112" s="2" t="inlineStr">
         <is>
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="F113" s="4" t="n">
-        <v>45772.94160647511</v>
+        <v>45773.91266737456</v>
       </c>
       <c r="G113" s="2" t="inlineStr">
         <is>
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="F114" s="4" t="n">
-        <v>45772.94160649356</v>
+        <v>45773.91266739279</v>
       </c>
       <c r="G114" s="2" t="inlineStr">
         <is>
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="F115" s="4" t="n">
-        <v>45772.94160651206</v>
+        <v>45773.91266741134</v>
       </c>
       <c r="G115" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
a litte less mess, worked on geometry, metadata json...
</commit_message>
<xml_diff>
--- a/projects/002_example_project__public/buildings/test_building_001/04_metrics/test_building_001_metrics.xlsx
+++ b/projects/002_example_project__public/buildings/test_building_001/04_metrics/test_building_001_metrics.xlsx
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>45773.9126282363</v>
+        <v>45774.51714972244</v>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="F3" s="4" t="n">
-        <v>45773.91262875602</v>
+        <v>45774.51715049539</v>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="F4" s="4" t="n">
-        <v>45773.91262928458</v>
+        <v>45774.5171510482</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="F5" s="4" t="n">
-        <v>45773.9126297759</v>
+        <v>45774.51715155634</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="F6" s="4" t="n">
-        <v>45773.91263029215</v>
+        <v>45774.51715210335</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F7" s="4" t="n">
-        <v>45773.9126308124</v>
+        <v>45774.51715266592</v>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="F8" s="4" t="n">
-        <v>45773.91263131925</v>
+        <v>45774.51715319938</v>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
@@ -761,7 +761,7 @@
         </is>
       </c>
       <c r="F9" s="4" t="n">
-        <v>45773.91263186544</v>
+        <v>45774.51715377426</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="F10" s="4" t="n">
-        <v>45773.91263241286</v>
+        <v>45774.51715433363</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="F11" s="4" t="n">
-        <v>45773.91263292476</v>
+        <v>45774.51715486211</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="F12" s="4" t="n">
-        <v>45773.91263342176</v>
+        <v>45774.51715539256</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="F13" s="4" t="n">
-        <v>45773.9126339538</v>
+        <v>45774.51715595108</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="F14" s="4" t="n">
-        <v>45773.91263447842</v>
+        <v>45774.51715651037</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="F15" s="4" t="n">
-        <v>45773.91263496603</v>
+        <v>45774.51715703134</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="F16" s="4" t="n">
-        <v>45773.91263545559</v>
+        <v>45774.51715754552</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="F17" s="4" t="n">
-        <v>45773.91263594059</v>
+        <v>45774.51715805998</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="F18" s="4" t="n">
-        <v>45773.9126364302</v>
+        <v>45774.51715857739</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="F19" s="4" t="n">
-        <v>45773.91263692616</v>
+        <v>45774.51715910548</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="F20" s="4" t="n">
-        <v>45773.91263742017</v>
+        <v>45774.51715972563</v>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="F21" s="4" t="n">
-        <v>45773.9126379204</v>
+        <v>45774.5171603612</v>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="F22" s="4" t="n">
-        <v>45773.91263846097</v>
+        <v>45774.51716100444</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
@@ -1223,7 +1223,7 @@
         </is>
       </c>
       <c r="F23" s="4" t="n">
-        <v>45773.91263906474</v>
+        <v>45774.51716164342</v>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="F24" s="4" t="n">
-        <v>45773.91263967872</v>
+        <v>45774.51716231722</v>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="F25" s="4" t="n">
-        <v>45773.91264050485</v>
+        <v>45774.51716316248</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="F26" s="4" t="n">
-        <v>45773.91264269219</v>
+        <v>45774.51716414197</v>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>45773.91264364828</v>
+        <v>45774.51716510336</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
@@ -1388,7 +1388,7 @@
         </is>
       </c>
       <c r="F28" s="4" t="n">
-        <v>45773.91264439347</v>
+        <v>45774.5171659611</v>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
@@ -1421,7 +1421,7 @@
         </is>
       </c>
       <c r="F29" s="4" t="n">
-        <v>45773.9126453016</v>
+        <v>45774.51716695887</v>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="F30" s="4" t="n">
-        <v>45773.91264620119</v>
+        <v>45774.51716788067</v>
       </c>
       <c r="G30" s="2" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="F31" s="4" t="n">
-        <v>45773.91264696535</v>
+        <v>45774.51716863063</v>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F32" s="4" t="n">
-        <v>45773.91264752953</v>
+        <v>45774.51716917584</v>
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
@@ -1556,7 +1556,7 @@
         </is>
       </c>
       <c r="F33" s="4" t="n">
-        <v>45773.91264802944</v>
+        <v>45774.51716970009</v>
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="F34" s="4" t="n">
-        <v>45773.91264854317</v>
+        <v>45774.51717024361</v>
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="F35" s="4" t="n">
-        <v>45773.91264905013</v>
+        <v>45774.51717077286</v>
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         </is>
       </c>
       <c r="F36" s="4" t="n">
-        <v>45773.91264955245</v>
+        <v>45774.51717126879</v>
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
         </is>
       </c>
       <c r="F37" s="4" t="n">
-        <v>45773.91265006747</v>
+        <v>45774.51717177722</v>
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
@@ -1721,7 +1721,7 @@
         </is>
       </c>
       <c r="F38" s="4" t="n">
-        <v>45773.91265058192</v>
+        <v>45774.5171722889</v>
       </c>
       <c r="G38" s="2" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="F39" s="4" t="n">
-        <v>45773.91265107925</v>
+        <v>45774.51717278786</v>
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="F40" s="4" t="n">
-        <v>45773.91265159703</v>
+        <v>45774.51717330979</v>
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="F41" s="4" t="n">
-        <v>45773.91265211068</v>
+        <v>45774.51717382465</v>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="F42" s="4" t="n">
-        <v>45773.91265261287</v>
+        <v>45774.5171743219</v>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F43" s="4" t="n">
-        <v>45773.91265311016</v>
+        <v>45774.51717483098</v>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="F44" s="4" t="n">
-        <v>45773.91265360954</v>
+        <v>45774.51717533365</v>
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="F45" s="4" t="n">
-        <v>45773.91265410541</v>
+        <v>45774.5171758264</v>
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="F46" s="4" t="n">
-        <v>45773.91265460493</v>
+        <v>45774.51717632551</v>
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="F47" s="4" t="n">
-        <v>45773.91265509769</v>
+        <v>45774.51717681944</v>
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="F48" s="4" t="n">
-        <v>45773.91265559488</v>
+        <v>45774.51717731839</v>
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="F49" s="4" t="n">
-        <v>45773.91265615854</v>
+        <v>45774.51717788205</v>
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="F50" s="4" t="n">
-        <v>45773.91265693743</v>
+        <v>45774.51717849063</v>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="F51" s="4" t="n">
-        <v>45773.91265758663</v>
+        <v>45774.51717910669</v>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
@@ -2188,7 +2188,7 @@
         </is>
       </c>
       <c r="F52" s="4" t="n">
-        <v>45773.91265816594</v>
+        <v>45774.5171796872</v>
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
@@ -2225,7 +2225,7 @@
         </is>
       </c>
       <c r="F53" s="4" t="n">
-        <v>45773.91265886419</v>
+        <v>45774.51718033342</v>
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="F54" s="4" t="n">
-        <v>45773.91265960685</v>
+        <v>45774.51718098157</v>
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="F55" s="4" t="n">
-        <v>45773.91266012248</v>
+        <v>45774.51718151278</v>
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="F56" s="4" t="n">
-        <v>45773.91266062044</v>
+        <v>45774.51718201656</v>
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
@@ -2361,7 +2361,7 @@
         </is>
       </c>
       <c r="F57" s="4" t="n">
-        <v>45773.9126611179</v>
+        <v>45774.51718251223</v>
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
@@ -2394,7 +2394,7 @@
         </is>
       </c>
       <c r="F58" s="4" t="n">
-        <v>45773.91266163401</v>
+        <v>45774.51718302231</v>
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="F59" s="4" t="n">
-        <v>45773.91266163419</v>
+        <v>45774.51718302244</v>
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="E60" s="2" t="inlineStr"/>
       <c r="F60" s="4" t="n">
-        <v>45773.91266240962</v>
+        <v>45774.51718373374</v>
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="E61" s="2" t="inlineStr"/>
       <c r="F61" s="4" t="n">
-        <v>45773.91266325641</v>
+        <v>45774.51718454775</v>
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
@@ -2514,7 +2514,7 @@
         </is>
       </c>
       <c r="F62" s="4" t="n">
-        <v>45773.91266387749</v>
+        <v>45774.51718513152</v>
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
@@ -2547,7 +2547,7 @@
         </is>
       </c>
       <c r="F63" s="4" t="n">
-        <v>45773.91266387759</v>
+        <v>45774.51718513161</v>
       </c>
       <c r="G63" s="2" t="inlineStr">
         <is>
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="F64" s="4" t="n">
-        <v>45773.91266387761</v>
+        <v>45774.51718513163</v>
       </c>
       <c r="G64" s="2" t="inlineStr">
         <is>
@@ -2613,7 +2613,7 @@
         </is>
       </c>
       <c r="F65" s="4" t="n">
-        <v>45773.91266387763</v>
+        <v>45774.51718513164</v>
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
@@ -2646,7 +2646,7 @@
         </is>
       </c>
       <c r="F66" s="4" t="n">
-        <v>45773.91266387764</v>
+        <v>45774.51718513166</v>
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
@@ -2679,7 +2679,7 @@
         </is>
       </c>
       <c r="F67" s="4" t="n">
-        <v>45773.91266387765</v>
+        <v>45774.51718513167</v>
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="F68" s="4" t="n">
-        <v>45773.91266387767</v>
+        <v>45774.51718513168</v>
       </c>
       <c r="G68" s="2" t="inlineStr">
         <is>
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="F69" s="4" t="n">
-        <v>45773.91266387773</v>
+        <v>45774.51718513175</v>
       </c>
       <c r="G69" s="2" t="inlineStr">
         <is>
@@ -2778,7 +2778,7 @@
         </is>
       </c>
       <c r="F70" s="4" t="n">
-        <v>45773.91266387775</v>
+        <v>45774.51718513176</v>
       </c>
       <c r="G70" s="2" t="inlineStr">
         <is>
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="F71" s="4" t="n">
-        <v>45773.91266387777</v>
+        <v>45774.51718513177</v>
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
@@ -2844,7 +2844,7 @@
         </is>
       </c>
       <c r="F72" s="4" t="n">
-        <v>45773.91266387777</v>
+        <v>45774.51718513178</v>
       </c>
       <c r="G72" s="2" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="F73" s="4" t="n">
-        <v>45773.91266387779</v>
+        <v>45774.51718513179</v>
       </c>
       <c r="G73" s="2" t="inlineStr">
         <is>
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="F74" s="4" t="n">
-        <v>45773.91266443131</v>
+        <v>45774.51718566574</v>
       </c>
       <c r="G74" s="2" t="inlineStr">
         <is>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="F75" s="4" t="n">
-        <v>45773.91266443139</v>
+        <v>45774.51718566582</v>
       </c>
       <c r="G75" s="2" t="inlineStr">
         <is>
@@ -2976,7 +2976,7 @@
         </is>
       </c>
       <c r="F76" s="4" t="n">
-        <v>45773.9126644314</v>
+        <v>45774.51718566583</v>
       </c>
       <c r="G76" s="2" t="inlineStr">
         <is>
@@ -3009,7 +3009,7 @@
         </is>
       </c>
       <c r="F77" s="4" t="n">
-        <v>45773.91266443141</v>
+        <v>45774.51718566584</v>
       </c>
       <c r="G77" s="2" t="inlineStr">
         <is>
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="F78" s="4" t="n">
-        <v>45773.91266443142</v>
+        <v>45774.51718566586</v>
       </c>
       <c r="G78" s="2" t="inlineStr">
         <is>
@@ -3075,7 +3075,7 @@
         </is>
       </c>
       <c r="F79" s="4" t="n">
-        <v>45773.91266443144</v>
+        <v>45774.51718566587</v>
       </c>
       <c r="G79" s="2" t="inlineStr">
         <is>
@@ -3108,7 +3108,7 @@
         </is>
       </c>
       <c r="F80" s="4" t="n">
-        <v>45773.91266443145</v>
+        <v>45774.51718566588</v>
       </c>
       <c r="G80" s="2" t="inlineStr">
         <is>
@@ -3141,7 +3141,7 @@
         </is>
       </c>
       <c r="F81" s="4" t="n">
-        <v>45773.91266443146</v>
+        <v>45774.51718566588</v>
       </c>
       <c r="G81" s="2" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
         </is>
       </c>
       <c r="F82" s="4" t="n">
-        <v>45773.91266443147</v>
+        <v>45774.51718566589</v>
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="F83" s="4" t="n">
-        <v>45773.91266443148</v>
+        <v>45774.5171856659</v>
       </c>
       <c r="G83" s="2" t="inlineStr">
         <is>
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="F84" s="4" t="n">
-        <v>45773.9126644315</v>
+        <v>45774.51718566591</v>
       </c>
       <c r="G84" s="2" t="inlineStr">
         <is>
@@ -3273,7 +3273,7 @@
         </is>
       </c>
       <c r="F85" s="4" t="n">
-        <v>45773.9126644315</v>
+        <v>45774.51718566593</v>
       </c>
       <c r="G85" s="2" t="inlineStr">
         <is>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="E86" s="2" t="inlineStr"/>
       <c r="F86" s="4" t="n">
-        <v>45773.91266565309</v>
+        <v>45774.51718689167</v>
       </c>
       <c r="G86" s="2" t="inlineStr">
         <is>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="E87" s="2" t="inlineStr"/>
       <c r="F87" s="4" t="n">
-        <v>45773.9126662257</v>
+        <v>45774.51718746465</v>
       </c>
       <c r="G87" s="2" t="inlineStr">
         <is>
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="F88" s="4" t="n">
-        <v>45773.91266689355</v>
+        <v>45774.5171884009</v>
       </c>
       <c r="G88" s="2" t="inlineStr">
         <is>
@@ -3393,7 +3393,7 @@
         </is>
       </c>
       <c r="F89" s="4" t="n">
-        <v>45773.91266691661</v>
+        <v>45774.51718842874</v>
       </c>
       <c r="G89" s="2" t="inlineStr">
         <is>
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="F90" s="4" t="n">
-        <v>45773.91266693729</v>
+        <v>45774.51718845382</v>
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
@@ -3459,7 +3459,7 @@
         </is>
       </c>
       <c r="F91" s="4" t="n">
-        <v>45773.91266695712</v>
+        <v>45774.51718847759</v>
       </c>
       <c r="G91" s="2" t="inlineStr">
         <is>
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="F92" s="4" t="n">
-        <v>45773.91266697707</v>
+        <v>45774.51718850067</v>
       </c>
       <c r="G92" s="2" t="inlineStr">
         <is>
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="F93" s="4" t="n">
-        <v>45773.91266699648</v>
+        <v>45774.51718852334</v>
       </c>
       <c r="G93" s="2" t="inlineStr">
         <is>
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="F94" s="4" t="n">
-        <v>45773.91266701606</v>
+        <v>45774.51718854681</v>
       </c>
       <c r="G94" s="2" t="inlineStr">
         <is>
@@ -3591,7 +3591,7 @@
         </is>
       </c>
       <c r="F95" s="4" t="n">
-        <v>45773.91266703577</v>
+        <v>45774.51718856983</v>
       </c>
       <c r="G95" s="2" t="inlineStr">
         <is>
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="F96" s="4" t="n">
-        <v>45773.91266705455</v>
+        <v>45774.51718859068</v>
       </c>
       <c r="G96" s="2" t="inlineStr">
         <is>
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="F97" s="4" t="n">
-        <v>45773.91266707351</v>
+        <v>45774.51718861112</v>
       </c>
       <c r="G97" s="2" t="inlineStr">
         <is>
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="F98" s="4" t="n">
-        <v>45773.9126670922</v>
+        <v>45774.51718863122</v>
       </c>
       <c r="G98" s="2" t="inlineStr">
         <is>
@@ -3723,7 +3723,7 @@
         </is>
       </c>
       <c r="F99" s="4" t="n">
-        <v>45773.91266711154</v>
+        <v>45774.51718865108</v>
       </c>
       <c r="G99" s="2" t="inlineStr">
         <is>
@@ -3756,7 +3756,7 @@
         </is>
       </c>
       <c r="F100" s="4" t="n">
-        <v>45773.91266713069</v>
+        <v>45774.51718867097</v>
       </c>
       <c r="G100" s="2" t="inlineStr">
         <is>
@@ -3789,7 +3789,7 @@
         </is>
       </c>
       <c r="F101" s="4" t="n">
-        <v>45773.91266714923</v>
+        <v>45774.51718869057</v>
       </c>
       <c r="G101" s="2" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F102" s="4" t="n">
-        <v>45773.91266716787</v>
+        <v>45774.5171887101</v>
       </c>
       <c r="G102" s="2" t="inlineStr">
         <is>
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="F103" s="4" t="n">
-        <v>45773.91266718714</v>
+        <v>45774.51718873045</v>
       </c>
       <c r="G103" s="2" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
         </is>
       </c>
       <c r="F104" s="4" t="n">
-        <v>45773.91266720785</v>
+        <v>45774.51718874928</v>
       </c>
       <c r="G104" s="2" t="inlineStr">
         <is>
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="F105" s="4" t="n">
-        <v>45773.91266722714</v>
+        <v>45774.51718876838</v>
       </c>
       <c r="G105" s="2" t="inlineStr">
         <is>
@@ -3954,7 +3954,7 @@
         </is>
       </c>
       <c r="F106" s="4" t="n">
-        <v>45773.91266724555</v>
+        <v>45774.51718878747</v>
       </c>
       <c r="G106" s="2" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
         </is>
       </c>
       <c r="F107" s="4" t="n">
-        <v>45773.91266726385</v>
+        <v>45774.51718880704</v>
       </c>
       <c r="G107" s="2" t="inlineStr">
         <is>
@@ -4020,7 +4020,7 @@
         </is>
       </c>
       <c r="F108" s="4" t="n">
-        <v>45773.91266728217</v>
+        <v>45774.5171888262</v>
       </c>
       <c r="G108" s="2" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
         </is>
       </c>
       <c r="F109" s="4" t="n">
-        <v>45773.91266730044</v>
+        <v>45774.51718884545</v>
       </c>
       <c r="G109" s="2" t="inlineStr">
         <is>
@@ -4086,7 +4086,7 @@
         </is>
       </c>
       <c r="F110" s="4" t="n">
-        <v>45773.9126673189</v>
+        <v>45774.51718886448</v>
       </c>
       <c r="G110" s="2" t="inlineStr">
         <is>
@@ -4119,7 +4119,7 @@
         </is>
       </c>
       <c r="F111" s="4" t="n">
-        <v>45773.91266733744</v>
+        <v>45774.51718888384</v>
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="F112" s="4" t="n">
-        <v>45773.91266735609</v>
+        <v>45774.5171889031</v>
       </c>
       <c r="G112" s="2" t="inlineStr">
         <is>
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="F113" s="4" t="n">
-        <v>45773.91266737456</v>
+        <v>45774.51718892213</v>
       </c>
       <c r="G113" s="2" t="inlineStr">
         <is>
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="F114" s="4" t="n">
-        <v>45773.91266739279</v>
+        <v>45774.51718894127</v>
       </c>
       <c r="G114" s="2" t="inlineStr">
         <is>
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="F115" s="4" t="n">
-        <v>45773.91266741134</v>
+        <v>45774.51718896026</v>
       </c>
       <c r="G115" s="2" t="inlineStr">
         <is>

</xml_diff>